<commit_message>
Bugfixes and tweak to how Snippets chart exports
</commit_message>
<xml_diff>
--- a/Jsafety_Sweeps.xlsx
+++ b/Jsafety_Sweeps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepos\MATLAB\NHP_Patch_Experiments\+charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE42E1-2224-4107-A0FD-CF8A3634032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2A24D-DA62-4E09-B291-862155823EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="58275" yWindow="19875" windowWidth="20565" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5015,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06071E07-0FE2-4EBD-9652-D997CD54C11C}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L97" sqref="L97"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>